<commit_message>
Excel data input, test results and advanced search
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BrowserConfiguration" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="AdvancedSearchValues" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="109">
   <si>
     <t>PageURL</t>
   </si>
@@ -37,6 +37,312 @@
   </si>
   <si>
     <t>To change browser, enter one of the ID's into the BrowserID section at A:2</t>
+  </si>
+  <si>
+    <t>Postcode</t>
+  </si>
+  <si>
+    <t>Used</t>
+  </si>
+  <si>
+    <t>Nearly New</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Min Price</t>
+  </si>
+  <si>
+    <t>Max Price</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>Make</t>
+  </si>
+  <si>
+    <t>M84NP</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Searh Key</t>
+  </si>
+  <si>
+    <t>Searches by partial text value (e.g. can enter "Chev" for "Chevrolet")</t>
+  </si>
+  <si>
+    <t>Text is inserted as entered in this sheet</t>
+  </si>
+  <si>
+    <t>Selects value from a list, check the "Distance Value List"</t>
+  </si>
+  <si>
+    <t>Simply toggles the "Used" checkbox from selected to unselected if this value is "yes"</t>
+  </si>
+  <si>
+    <t>Simply toggles the "Nearly New" checkbox from selected to unselected if this value is "yes"</t>
+  </si>
+  <si>
+    <t>Simply toggles the "New" checkbox from selected to unselected if this value is "yes"</t>
+  </si>
+  <si>
+    <t>Selects value from a list, check the "Min Price List"</t>
+  </si>
+  <si>
+    <t>Selects value from a list, check the "Max Price List"</t>
+  </si>
+  <si>
+    <t>Distance Value List</t>
+  </si>
+  <si>
+    <t>Distance (any)</t>
+  </si>
+  <si>
+    <t>Within 1 mile</t>
+  </si>
+  <si>
+    <t>Within 5 miles</t>
+  </si>
+  <si>
+    <t>Within 10 miles</t>
+  </si>
+  <si>
+    <t>Within 15 miles</t>
+  </si>
+  <si>
+    <t>Within 20 miles</t>
+  </si>
+  <si>
+    <t>Within 25 miles</t>
+  </si>
+  <si>
+    <t>Within 30 miles</t>
+  </si>
+  <si>
+    <t>Within 35 miles</t>
+  </si>
+  <si>
+    <t>Within 40 miles</t>
+  </si>
+  <si>
+    <t>Within 45 miles</t>
+  </si>
+  <si>
+    <t>Within 50 miles</t>
+  </si>
+  <si>
+    <t>Within 55 miles</t>
+  </si>
+  <si>
+    <t>Within 60 miles</t>
+  </si>
+  <si>
+    <t>Within 70 miles</t>
+  </si>
+  <si>
+    <t>Within 80 miles</t>
+  </si>
+  <si>
+    <t>Within 90 miles</t>
+  </si>
+  <si>
+    <t>Within 100 miles</t>
+  </si>
+  <si>
+    <t>Within 200 miles</t>
+  </si>
+  <si>
+    <t>National</t>
+  </si>
+  <si>
+    <t>Enter the left hand value into the "Distance" to apply it.</t>
+  </si>
+  <si>
+    <t>For national, leave the "Distance" empty.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>From £0</t>
+  </si>
+  <si>
+    <t>From £500</t>
+  </si>
+  <si>
+    <t>From £1,000</t>
+  </si>
+  <si>
+    <t>From £1,500</t>
+  </si>
+  <si>
+    <t>From £2,000</t>
+  </si>
+  <si>
+    <t>From £2,500</t>
+  </si>
+  <si>
+    <t>From £3,000</t>
+  </si>
+  <si>
+    <t>From £3,500</t>
+  </si>
+  <si>
+    <t>From £4,000</t>
+  </si>
+  <si>
+    <t>From £4,500</t>
+  </si>
+  <si>
+    <t>From £5,000</t>
+  </si>
+  <si>
+    <t>From £5,500</t>
+  </si>
+  <si>
+    <t>From £6,000</t>
+  </si>
+  <si>
+    <t>From £6,500</t>
+  </si>
+  <si>
+    <t>From £7,000</t>
+  </si>
+  <si>
+    <t>From £7,500</t>
+  </si>
+  <si>
+    <t>From £8,000</t>
+  </si>
+  <si>
+    <t>From £8,500</t>
+  </si>
+  <si>
+    <t>From £9,000</t>
+  </si>
+  <si>
+    <t>From £9,500</t>
+  </si>
+  <si>
+    <t>From £10,000</t>
+  </si>
+  <si>
+    <t>From £11,000</t>
+  </si>
+  <si>
+    <t>From £12,000</t>
+  </si>
+  <si>
+    <t>From £13,000</t>
+  </si>
+  <si>
+    <t>From £14,000</t>
+  </si>
+  <si>
+    <t>From £15,000</t>
+  </si>
+  <si>
+    <t>From £16,000</t>
+  </si>
+  <si>
+    <t>From £17,000</t>
+  </si>
+  <si>
+    <t>From £18,000</t>
+  </si>
+  <si>
+    <t>From £19,000</t>
+  </si>
+  <si>
+    <t>From £20,000</t>
+  </si>
+  <si>
+    <t>From £22,500</t>
+  </si>
+  <si>
+    <t>From £25,000</t>
+  </si>
+  <si>
+    <t>From £27,500</t>
+  </si>
+  <si>
+    <t>From £30,000</t>
+  </si>
+  <si>
+    <t>From £35,000</t>
+  </si>
+  <si>
+    <t>From £40,000</t>
+  </si>
+  <si>
+    <t>From £45,000</t>
+  </si>
+  <si>
+    <t>From £50,000</t>
+  </si>
+  <si>
+    <t>From £55,000</t>
+  </si>
+  <si>
+    <t>From £60,000</t>
+  </si>
+  <si>
+    <t>From £65,000</t>
+  </si>
+  <si>
+    <t>From £70,000</t>
+  </si>
+  <si>
+    <t>From £75,000</t>
+  </si>
+  <si>
+    <t>From £100,000</t>
+  </si>
+  <si>
+    <t>From £250,000</t>
+  </si>
+  <si>
+    <t>From £500,000</t>
+  </si>
+  <si>
+    <t>From £1,000,000</t>
+  </si>
+  <si>
+    <t>From £2,000,000</t>
+  </si>
+  <si>
+    <t>Price List Values (2)</t>
+  </si>
+  <si>
+    <t>Price List Values (1)</t>
+  </si>
+  <si>
+    <t>For "Min price (any)", leave the "Min Price" or "Max Price" empty.</t>
+  </si>
+  <si>
+    <t>Enter the left hand value into the "Min Price" or "Max Price" to apply it.</t>
+  </si>
+  <si>
+    <t>Min/Max price (any)</t>
+  </si>
+  <si>
+    <t>Note: Min price can be anything, but max price MUST be more than or equal to min price.</t>
+  </si>
+  <si>
+    <t>Note: If there is only one vehicle available while inputting the values, all inputs will be ignored and a search will run.</t>
+  </si>
+  <si>
+    <t>Postcode (*)</t>
+  </si>
+  <si>
+    <t>(*) = Required, must not be empty or search will fail.</t>
   </si>
 </sst>
 </file>
@@ -60,7 +366,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -85,8 +391,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -163,13 +475,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
@@ -179,6 +540,48 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -484,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,50 +900,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -555,12 +958,1406 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:W56"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="10" width="12.42578125" customWidth="1"/>
+    <col min="20" max="20" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="21"/>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="21"/>
+      <c r="S4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="21"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="18"/>
+      <c r="K9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="15"/>
+      <c r="K10" s="5">
+        <v>1500</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="15"/>
+      <c r="K11" s="5">
+        <v>1</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="15"/>
+      <c r="K12" s="5">
+        <v>5</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="15"/>
+      <c r="K13" s="5">
+        <v>10</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="K14" s="5">
+        <v>15</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="K15" s="5">
+        <v>20</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="K16" s="5">
+        <v>25</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="K17" s="5">
+        <v>30</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="K18" s="5">
+        <v>35</v>
+      </c>
+      <c r="L18" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K19" s="5">
+        <v>40</v>
+      </c>
+      <c r="L19" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K20" s="5">
+        <v>45</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K21" s="5">
+        <v>50</v>
+      </c>
+      <c r="L21" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K22" s="5">
+        <v>55</v>
+      </c>
+      <c r="L22" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K23" s="5">
+        <v>60</v>
+      </c>
+      <c r="L23" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K24" s="5">
+        <v>70</v>
+      </c>
+      <c r="L24" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K25" s="5">
+        <v>80</v>
+      </c>
+      <c r="L25" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K26" s="5">
+        <v>90</v>
+      </c>
+      <c r="L26" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K27" s="5">
+        <v>100</v>
+      </c>
+      <c r="L27" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K28" s="5">
+        <v>200</v>
+      </c>
+      <c r="L28" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K29" s="5"/>
+      <c r="L29" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+    </row>
+    <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K30" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K31" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="I33" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="Q33" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="R33" s="9"/>
+      <c r="S33" s="9"/>
+      <c r="T33" s="9"/>
+      <c r="U33" s="9"/>
+      <c r="V33" s="9"/>
+      <c r="W33" s="9"/>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="I34" s="1">
+        <v>9500</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="Q34" s="1">
+        <v>55000</v>
+      </c>
+      <c r="R34" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="S34" s="8"/>
+      <c r="T34" s="8"/>
+      <c r="U34" s="8"/>
+      <c r="V34" s="8"/>
+      <c r="W34" s="8"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>0</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="I35" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="Q35" s="1">
+        <v>60000</v>
+      </c>
+      <c r="R35" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="S35" s="8"/>
+      <c r="T35" s="8"/>
+      <c r="U35" s="8"/>
+      <c r="V35" s="8"/>
+      <c r="W35" s="8"/>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>500</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="I36" s="1">
+        <v>11000</v>
+      </c>
+      <c r="J36" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="Q36" s="1">
+        <v>65000</v>
+      </c>
+      <c r="R36" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="S36" s="8"/>
+      <c r="T36" s="8"/>
+      <c r="U36" s="8"/>
+      <c r="V36" s="8"/>
+      <c r="W36" s="8"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="I37" s="1">
+        <v>12000</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="Q37" s="1">
+        <v>70000</v>
+      </c>
+      <c r="R37" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="S37" s="8"/>
+      <c r="T37" s="8"/>
+      <c r="U37" s="8"/>
+      <c r="V37" s="8"/>
+      <c r="W37" s="8"/>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>1500</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="I38" s="1">
+        <v>13000</v>
+      </c>
+      <c r="J38" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="Q38" s="1">
+        <v>75000</v>
+      </c>
+      <c r="R38" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="S38" s="8"/>
+      <c r="T38" s="8"/>
+      <c r="U38" s="8"/>
+      <c r="V38" s="8"/>
+      <c r="W38" s="8"/>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="I39" s="1">
+        <v>14000</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="Q39" s="1">
+        <v>100000</v>
+      </c>
+      <c r="R39" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="S39" s="8"/>
+      <c r="T39" s="8"/>
+      <c r="U39" s="8"/>
+      <c r="V39" s="8"/>
+      <c r="W39" s="8"/>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>2500</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="I40" s="1">
+        <v>15000</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="Q40" s="1">
+        <v>250000</v>
+      </c>
+      <c r="R40" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="S40" s="8"/>
+      <c r="T40" s="8"/>
+      <c r="U40" s="8"/>
+      <c r="V40" s="8"/>
+      <c r="W40" s="8"/>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>3000</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="I41" s="1">
+        <v>16000</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="Q41" s="1">
+        <v>500000</v>
+      </c>
+      <c r="R41" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="S41" s="8"/>
+      <c r="T41" s="8"/>
+      <c r="U41" s="8"/>
+      <c r="V41" s="8"/>
+      <c r="W41" s="8"/>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>3500</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="I42" s="1">
+        <v>17000</v>
+      </c>
+      <c r="J42" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="Q42" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="R42" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="S42" s="8"/>
+      <c r="T42" s="8"/>
+      <c r="U42" s="8"/>
+      <c r="V42" s="8"/>
+      <c r="W42" s="8"/>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>4000</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="I43" s="1">
+        <v>18000</v>
+      </c>
+      <c r="J43" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="Q43" s="1">
+        <v>2000000</v>
+      </c>
+      <c r="R43" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="S43" s="8"/>
+      <c r="T43" s="8"/>
+      <c r="U43" s="8"/>
+      <c r="V43" s="8"/>
+      <c r="W43" s="8"/>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>4500</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="I44" s="1">
+        <v>19000</v>
+      </c>
+      <c r="J44" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="8"/>
+      <c r="S44" s="8"/>
+      <c r="T44" s="8"/>
+      <c r="U44" s="8"/>
+      <c r="V44" s="8"/>
+      <c r="W44" s="8"/>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>5000</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="I45" s="1">
+        <v>20000</v>
+      </c>
+      <c r="J45" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="8"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="8"/>
+      <c r="S45" s="8"/>
+      <c r="T45" s="8"/>
+      <c r="U45" s="8"/>
+      <c r="V45" s="8"/>
+      <c r="W45" s="8"/>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>5500</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="I46" s="1">
+        <v>22500</v>
+      </c>
+      <c r="J46" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="8"/>
+      <c r="O46" s="8"/>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="8"/>
+      <c r="S46" s="8"/>
+      <c r="T46" s="8"/>
+      <c r="U46" s="8"/>
+      <c r="V46" s="8"/>
+      <c r="W46" s="8"/>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>6000</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="I47" s="1">
+        <v>25000</v>
+      </c>
+      <c r="J47" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="8"/>
+      <c r="N47" s="8"/>
+      <c r="O47" s="8"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="8"/>
+      <c r="S47" s="8"/>
+      <c r="T47" s="8"/>
+      <c r="U47" s="8"/>
+      <c r="V47" s="8"/>
+      <c r="W47" s="8"/>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>6500</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="I48" s="1">
+        <v>27500</v>
+      </c>
+      <c r="J48" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="K48" s="8"/>
+      <c r="L48" s="8"/>
+      <c r="M48" s="8"/>
+      <c r="N48" s="8"/>
+      <c r="O48" s="8"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="8"/>
+      <c r="S48" s="8"/>
+      <c r="T48" s="8"/>
+      <c r="U48" s="8"/>
+      <c r="V48" s="8"/>
+      <c r="W48" s="8"/>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>7000</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="I49" s="1">
+        <v>30000</v>
+      </c>
+      <c r="J49" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="8"/>
+      <c r="O49" s="8"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="8"/>
+      <c r="S49" s="8"/>
+      <c r="T49" s="8"/>
+      <c r="U49" s="8"/>
+      <c r="V49" s="8"/>
+      <c r="W49" s="8"/>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>7500</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="I50" s="1">
+        <v>35000</v>
+      </c>
+      <c r="J50" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="K50" s="8"/>
+      <c r="L50" s="8"/>
+      <c r="M50" s="8"/>
+      <c r="N50" s="8"/>
+      <c r="O50" s="8"/>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="8"/>
+      <c r="S50" s="8"/>
+      <c r="T50" s="8"/>
+      <c r="U50" s="8"/>
+      <c r="V50" s="8"/>
+      <c r="W50" s="8"/>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>8000</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="I51" s="1">
+        <v>40000</v>
+      </c>
+      <c r="J51" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="K51" s="8"/>
+      <c r="L51" s="8"/>
+      <c r="M51" s="8"/>
+      <c r="N51" s="8"/>
+      <c r="O51" s="8"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="8"/>
+      <c r="S51" s="8"/>
+      <c r="T51" s="8"/>
+      <c r="U51" s="8"/>
+      <c r="V51" s="8"/>
+      <c r="W51" s="8"/>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>8500</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="I52" s="1">
+        <v>45000</v>
+      </c>
+      <c r="J52" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="K52" s="8"/>
+      <c r="L52" s="8"/>
+      <c r="M52" s="8"/>
+      <c r="N52" s="8"/>
+      <c r="O52" s="8"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="8"/>
+      <c r="S52" s="8"/>
+      <c r="T52" s="8"/>
+      <c r="U52" s="8"/>
+      <c r="V52" s="8"/>
+      <c r="W52" s="8"/>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>9000</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="I53" s="1">
+        <v>50000</v>
+      </c>
+      <c r="J53" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="K53" s="8"/>
+      <c r="L53" s="8"/>
+      <c r="M53" s="8"/>
+      <c r="N53" s="8"/>
+      <c r="O53" s="8"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="8"/>
+      <c r="S53" s="8"/>
+      <c r="T53" s="8"/>
+      <c r="U53" s="8"/>
+      <c r="V53" s="8"/>
+      <c r="W53" s="8"/>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="I54" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J54" s="12"/>
+      <c r="K54" s="12"/>
+      <c r="L54" s="12"/>
+      <c r="M54" s="12"/>
+      <c r="N54" s="12"/>
+      <c r="O54" s="12"/>
+      <c r="Q54" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="R54" s="12"/>
+      <c r="S54" s="12"/>
+      <c r="T54" s="12"/>
+      <c r="U54" s="12"/>
+      <c r="V54" s="12"/>
+      <c r="W54" s="12"/>
+    </row>
+    <row r="55" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="12"/>
+      <c r="K55" s="12"/>
+      <c r="L55" s="12"/>
+      <c r="M55" s="12"/>
+      <c r="N55" s="12"/>
+      <c r="O55" s="12"/>
+      <c r="Q55" s="12"/>
+      <c r="R55" s="12"/>
+      <c r="S55" s="12"/>
+      <c r="T55" s="12"/>
+      <c r="U55" s="12"/>
+      <c r="V55" s="12"/>
+      <c r="W55" s="12"/>
+    </row>
+    <row r="56" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="20"/>
+      <c r="H56" s="20"/>
+      <c r="I56" s="20"/>
+      <c r="J56" s="20"/>
+      <c r="K56" s="20"/>
+      <c r="L56" s="20"/>
+      <c r="M56" s="20"/>
+      <c r="N56" s="20"/>
+      <c r="O56" s="20"/>
+      <c r="P56" s="20"/>
+      <c r="Q56" s="20"/>
+      <c r="R56" s="20"/>
+      <c r="S56" s="20"/>
+      <c r="T56" s="20"/>
+      <c r="U56" s="20"/>
+      <c r="V56" s="20"/>
+      <c r="W56" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="106">
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="R49:W49"/>
+    <mergeCell ref="R50:W50"/>
+    <mergeCell ref="R51:W51"/>
+    <mergeCell ref="R52:W52"/>
+    <mergeCell ref="R53:W53"/>
+    <mergeCell ref="A56:W56"/>
+    <mergeCell ref="R44:W44"/>
+    <mergeCell ref="R45:W45"/>
+    <mergeCell ref="R46:W46"/>
+    <mergeCell ref="R47:W47"/>
+    <mergeCell ref="R48:W48"/>
+    <mergeCell ref="A54:G54"/>
+    <mergeCell ref="A55:G55"/>
+    <mergeCell ref="I54:O54"/>
+    <mergeCell ref="I55:O55"/>
+    <mergeCell ref="Q54:W54"/>
+    <mergeCell ref="Q55:W55"/>
+    <mergeCell ref="R38:W38"/>
+    <mergeCell ref="R37:W37"/>
+    <mergeCell ref="R36:W36"/>
+    <mergeCell ref="R35:W35"/>
+    <mergeCell ref="I33:O33"/>
+    <mergeCell ref="Q33:W33"/>
+    <mergeCell ref="J39:O39"/>
+    <mergeCell ref="J38:O38"/>
+    <mergeCell ref="J37:O37"/>
+    <mergeCell ref="J36:O36"/>
+    <mergeCell ref="J35:O35"/>
+    <mergeCell ref="R43:W43"/>
+    <mergeCell ref="R42:W42"/>
+    <mergeCell ref="R41:W41"/>
+    <mergeCell ref="R40:W40"/>
+    <mergeCell ref="R39:W39"/>
+    <mergeCell ref="J45:O45"/>
+    <mergeCell ref="J44:O44"/>
+    <mergeCell ref="J43:O43"/>
+    <mergeCell ref="J42:O42"/>
+    <mergeCell ref="J41:O41"/>
+    <mergeCell ref="J40:O40"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="J53:O53"/>
+    <mergeCell ref="R34:W34"/>
+    <mergeCell ref="J52:O52"/>
+    <mergeCell ref="J51:O51"/>
+    <mergeCell ref="J50:O50"/>
+    <mergeCell ref="J49:O49"/>
+    <mergeCell ref="J48:O48"/>
+    <mergeCell ref="J47:O47"/>
+    <mergeCell ref="J46:O46"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B45:G45"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="K31:Q31"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="J34:O34"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="L12:Q12"/>
+    <mergeCell ref="L11:Q11"/>
+    <mergeCell ref="L14:Q14"/>
+    <mergeCell ref="L15:Q15"/>
+    <mergeCell ref="K30:Q30"/>
+    <mergeCell ref="L18:Q18"/>
+    <mergeCell ref="L17:Q17"/>
+    <mergeCell ref="L16:Q16"/>
+    <mergeCell ref="L13:Q13"/>
+    <mergeCell ref="L24:Q24"/>
+    <mergeCell ref="L23:Q23"/>
+    <mergeCell ref="L22:Q22"/>
+    <mergeCell ref="L21:Q21"/>
+    <mergeCell ref="L20:Q20"/>
+    <mergeCell ref="L19:Q19"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="K9:Q9"/>
+    <mergeCell ref="L10:Q10"/>
+    <mergeCell ref="L29:Q29"/>
+    <mergeCell ref="L28:Q28"/>
+    <mergeCell ref="L27:Q27"/>
+    <mergeCell ref="L26:Q26"/>
+    <mergeCell ref="L25:Q25"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B15:I15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>